<commit_message>
AUTOMATION-58 CS Conbine sheets - add edits to tests based AUTOMATION-58 CS Conbine sheets - add edits to tests based on sprint 13.5
</commit_message>
<xml_diff>
--- a/src/test/resources/etalon/combinesheets/CS_004_preserveFormatting.xlsx
+++ b/src/test/resources/etalon/combinesheets/CS_004_preserveFormatting.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr/>
   <bookViews>
-    <workbookView xWindow="630" yWindow="555" windowWidth="27495" windowHeight="13485"/>
+    <workbookView xWindow="634" yWindow="557" windowWidth="27497" windowHeight="13483"/>
   </bookViews>
   <sheets>
     <sheet name="Combined data" sheetId="4" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="26">
   <si>
     <t>Column1</t>
   </si>
@@ -53,6 +53,51 @@
   </si>
   <si>
     <t>Row5</t>
+  </si>
+  <si>
+    <t>133</t>
+  </si>
+  <si>
+    <t>277</t>
+  </si>
+  <si>
+    <t>421</t>
+  </si>
+  <si>
+    <t>565</t>
+  </si>
+  <si>
+    <t>709</t>
+  </si>
+  <si>
+    <t>1863</t>
+  </si>
+  <si>
+    <t>3007</t>
+  </si>
+  <si>
+    <t>4151</t>
+  </si>
+  <si>
+    <t>5295</t>
+  </si>
+  <si>
+    <t>10219</t>
+  </si>
+  <si>
+    <t>960.5</t>
+  </si>
+  <si>
+    <t>1464.5</t>
+  </si>
+  <si>
+    <t>1968.5</t>
+  </si>
+  <si>
+    <t>2472.5</t>
+  </si>
+  <si>
+    <t>11976.5</t>
   </si>
 </sst>
 </file>
@@ -140,9 +185,8 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="1" fillId="6" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="2" fillId="6" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="3" fillId="6" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -379,417 +423,417 @@
   <dimension ref="A1:G18"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C30" sqref="C30"/>
+      <selection sqref="A1:G18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="12.640625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.35"/>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A1" s="1"/>
-      <c r="B1" s="2" t="s">
+    <row r="1" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A1" s="3"/>
+      <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="C1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="D1" s="2" t="s">
+      <c r="D1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="E1" s="2" t="s">
+      <c r="E1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="F1" s="2" t="s">
+      <c r="F1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="G1" s="3" t="s">
+      <c r="G1" s="2" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A2" s="2" t="s">
+    <row r="2" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="A2" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="B2" s="4">
+      <c r="B2" s="3">
         <v>1</v>
       </c>
-      <c r="C2" s="4">
+      <c r="C2" s="3">
         <v>2</v>
       </c>
-      <c r="D2" s="4">
+      <c r="D2" s="3">
         <v>10</v>
       </c>
-      <c r="E2" s="4">
+      <c r="E2" s="3">
         <v>20</v>
       </c>
-      <c r="F2" s="4">
+      <c r="F2" s="3">
         <v>100</v>
       </c>
-      <c r="G2" s="5">
-        <v>133</v>
-      </c>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A3" s="2" t="s">
+      <c r="G2" s="4" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="A3" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="B3" s="4">
+      <c r="B3" s="3">
         <v>3</v>
       </c>
-      <c r="C3" s="4">
+      <c r="C3" s="3">
         <v>4</v>
       </c>
-      <c r="D3" s="4">
+      <c r="D3" s="3">
         <v>30</v>
       </c>
-      <c r="E3" s="4">
+      <c r="E3" s="3">
         <v>40</v>
       </c>
-      <c r="F3" s="4">
+      <c r="F3" s="3">
         <v>200</v>
       </c>
-      <c r="G3" s="5">
-        <v>277</v>
-      </c>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A4" s="2" t="s">
+      <c r="G3" s="4" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="A4" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="B4" s="4">
+      <c r="B4" s="3">
         <v>5</v>
       </c>
-      <c r="C4" s="4">
+      <c r="C4" s="3">
         <v>6</v>
       </c>
-      <c r="D4" s="4">
+      <c r="D4" s="3">
         <v>50</v>
       </c>
-      <c r="E4" s="4">
+      <c r="E4" s="3">
         <v>60</v>
       </c>
-      <c r="F4" s="4">
+      <c r="F4" s="3">
         <v>300</v>
       </c>
-      <c r="G4" s="5">
-        <v>421</v>
-      </c>
-    </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A5" s="2" t="s">
+      <c r="G4" s="4" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="A5" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="B5" s="4">
+      <c r="B5" s="3">
         <v>7</v>
       </c>
-      <c r="C5" s="4">
+      <c r="C5" s="3">
         <v>8</v>
       </c>
-      <c r="D5" s="4">
+      <c r="D5" s="3">
         <v>70</v>
       </c>
-      <c r="E5" s="4">
+      <c r="E5" s="3">
         <v>80</v>
       </c>
-      <c r="F5" s="4">
+      <c r="F5" s="3">
         <v>400</v>
       </c>
-      <c r="G5" s="5">
-        <v>565</v>
-      </c>
-    </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A6" s="2" t="s">
+      <c r="G5" s="4" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="A6" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="B6" s="4">
+      <c r="B6" s="3">
         <v>9</v>
       </c>
-      <c r="C6" s="4">
+      <c r="C6" s="3">
         <v>10</v>
       </c>
-      <c r="D6" s="4">
+      <c r="D6" s="3">
         <v>90</v>
       </c>
-      <c r="E6" s="4">
+      <c r="E6" s="3">
         <v>100</v>
       </c>
-      <c r="F6" s="4">
+      <c r="F6" s="3">
         <v>500</v>
       </c>
-      <c r="G6" s="5">
-        <v>709</v>
-      </c>
-    </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A7" s="6"/>
-      <c r="B7" s="6" t="s">
+      <c r="G6" s="4" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="A7" s="5"/>
+      <c r="B7" s="5" t="s">
         <v>0</v>
       </c>
-      <c r="C7" s="6" t="s">
+      <c r="C7" s="5" t="s">
         <v>1</v>
       </c>
-      <c r="D7" s="6" t="s">
+      <c r="D7" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="E7" s="6" t="s">
+      <c r="E7" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="F7" s="6" t="s">
+      <c r="F7" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="G7" s="7" t="s">
+      <c r="G7" s="6" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A8" s="8" t="s">
+    <row r="8" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="A8" s="7" t="s">
         <v>6</v>
       </c>
-      <c r="B8" s="8">
+      <c r="B8" s="7">
         <v>11</v>
       </c>
-      <c r="C8" s="8">
+      <c r="C8" s="7">
         <v>22</v>
       </c>
-      <c r="D8" s="8">
+      <c r="D8" s="7">
         <v>310</v>
       </c>
-      <c r="E8" s="8">
+      <c r="E8" s="7">
         <v>420</v>
       </c>
-      <c r="F8" s="8">
+      <c r="F8" s="7">
         <v>1100</v>
       </c>
-      <c r="G8" s="9">
-        <v>1863</v>
-      </c>
-    </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A9" s="10" t="s">
+      <c r="G8" s="8" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="A9" s="9" t="s">
         <v>7</v>
       </c>
-      <c r="B9" s="10">
+      <c r="B9" s="9">
         <v>13</v>
       </c>
-      <c r="C9" s="10">
+      <c r="C9" s="9">
         <v>24</v>
       </c>
-      <c r="D9" s="10">
+      <c r="D9" s="9">
         <v>330</v>
       </c>
-      <c r="E9" s="10">
+      <c r="E9" s="9">
         <v>440</v>
       </c>
-      <c r="F9" s="10">
+      <c r="F9" s="9">
         <v>2200</v>
       </c>
-      <c r="G9" s="11">
-        <v>3007</v>
-      </c>
-    </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A10" s="8" t="s">
+      <c r="G9" s="10" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="A10" s="7" t="s">
         <v>8</v>
       </c>
-      <c r="B10" s="8">
+      <c r="B10" s="7">
         <v>15</v>
       </c>
-      <c r="C10" s="8">
+      <c r="C10" s="7">
         <v>26</v>
       </c>
-      <c r="D10" s="8">
+      <c r="D10" s="7">
         <v>350</v>
       </c>
-      <c r="E10" s="8">
+      <c r="E10" s="7">
         <v>460</v>
       </c>
-      <c r="F10" s="8">
+      <c r="F10" s="7">
         <v>3300</v>
       </c>
-      <c r="G10" s="9">
-        <v>4151</v>
-      </c>
-    </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A11" s="10" t="s">
+      <c r="G10" s="8" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="A11" s="9" t="s">
         <v>9</v>
       </c>
-      <c r="B11" s="10">
+      <c r="B11" s="9">
         <v>17</v>
       </c>
-      <c r="C11" s="10">
+      <c r="C11" s="9">
         <v>28</v>
       </c>
-      <c r="D11" s="10">
+      <c r="D11" s="9">
         <v>370</v>
       </c>
-      <c r="E11" s="10">
+      <c r="E11" s="9">
         <v>480</v>
       </c>
-      <c r="F11" s="10">
+      <c r="F11" s="9">
         <v>4400</v>
       </c>
-      <c r="G11" s="11">
-        <v>5295</v>
-      </c>
-    </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A12" s="8" t="s">
+      <c r="G11" s="10" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="A12" s="7" t="s">
         <v>10</v>
       </c>
-      <c r="B12" s="8">
+      <c r="B12" s="7">
         <v>19</v>
       </c>
-      <c r="C12" s="8">
+      <c r="C12" s="7">
         <v>210</v>
       </c>
-      <c r="D12" s="8">
+      <c r="D12" s="7">
         <v>390</v>
       </c>
-      <c r="E12" s="8">
+      <c r="E12" s="7">
         <v>4100</v>
       </c>
-      <c r="F12" s="8">
+      <c r="F12" s="7">
         <v>5500</v>
       </c>
-      <c r="G12" s="9">
-        <v>10219</v>
-      </c>
-    </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A13" s="4"/>
-      <c r="B13" s="2" t="s">
+      <c r="G12" s="8" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A13" s="3"/>
+      <c r="B13" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="C13" s="2" t="s">
+      <c r="C13" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="D13" s="2" t="s">
+      <c r="D13" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="E13" s="2" t="s">
+      <c r="E13" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="F13" s="2" t="s">
+      <c r="F13" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="G13" s="12" t="s">
+      <c r="G13" s="11" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A14" s="2" t="s">
+    <row r="14" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="A14" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="B14" s="4">
+      <c r="B14" s="3">
         <v>51</v>
       </c>
-      <c r="C14" s="4">
+      <c r="C14" s="3">
         <v>2.5</v>
       </c>
-      <c r="D14" s="4">
+      <c r="D14" s="3">
         <v>103</v>
       </c>
-      <c r="E14" s="4">
+      <c r="E14" s="3">
         <v>204</v>
       </c>
-      <c r="F14" s="4">
+      <c r="F14" s="3">
         <v>600</v>
       </c>
-      <c r="G14" s="13">
-        <v>960.5</v>
-      </c>
-    </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A15" s="2" t="s">
+      <c r="G14" s="12" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="A15" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="B15" s="4">
+      <c r="B15" s="3">
         <v>53</v>
       </c>
-      <c r="C15" s="4">
+      <c r="C15" s="3">
         <v>4.5</v>
       </c>
-      <c r="D15" s="4">
+      <c r="D15" s="3">
         <v>303</v>
       </c>
-      <c r="E15" s="4">
+      <c r="E15" s="3">
         <v>404</v>
       </c>
-      <c r="F15" s="4">
+      <c r="F15" s="3">
         <v>700</v>
       </c>
-      <c r="G15" s="13">
-        <v>1464.5</v>
-      </c>
-    </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A16" s="2" t="s">
+      <c r="G15" s="12" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="A16" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="B16" s="4">
+      <c r="B16" s="3">
         <v>55</v>
       </c>
-      <c r="C16" s="4">
+      <c r="C16" s="3">
         <v>6.5</v>
       </c>
-      <c r="D16" s="4">
+      <c r="D16" s="3">
         <v>503</v>
       </c>
-      <c r="E16" s="4">
+      <c r="E16" s="3">
         <v>604</v>
       </c>
-      <c r="F16" s="4">
+      <c r="F16" s="3">
         <v>800</v>
       </c>
-      <c r="G16" s="13">
-        <v>1968.5</v>
-      </c>
-    </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A17" s="2" t="s">
+      <c r="G16" s="12" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="A17" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="B17" s="4">
+      <c r="B17" s="3">
         <v>57</v>
       </c>
-      <c r="C17" s="4">
+      <c r="C17" s="3">
         <v>8.5</v>
       </c>
-      <c r="D17" s="4">
+      <c r="D17" s="3">
         <v>703</v>
       </c>
-      <c r="E17" s="4">
+      <c r="E17" s="3">
         <v>804</v>
       </c>
-      <c r="F17" s="4">
+      <c r="F17" s="3">
         <v>900</v>
       </c>
-      <c r="G17" s="13">
-        <v>2472.5</v>
-      </c>
-    </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A18" s="2" t="s">
+      <c r="G17" s="12" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="A18" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="B18" s="4">
+      <c r="B18" s="3">
         <v>59</v>
       </c>
-      <c r="C18" s="4">
+      <c r="C18" s="3">
         <v>10.5</v>
       </c>
-      <c r="D18" s="4">
+      <c r="D18" s="3">
         <v>903</v>
       </c>
-      <c r="E18" s="4">
+      <c r="E18" s="3">
         <v>1004</v>
       </c>
-      <c r="F18" s="4">
+      <c r="F18" s="3">
         <v>10000</v>
       </c>
-      <c r="G18" s="13">
-        <v>11976.5</v>
+      <c r="G18" s="12" t="s">
+        <v>25</v>
       </c>
     </row>
   </sheetData>

</xml_diff>